<commit_message>
Added DataDrivenLoginTest, and made some minor changes.
</commit_message>
<xml_diff>
--- a/testdata/OpenCart_LoginData.xlsx
+++ b/testdata/OpenCart_LoginData.xlsx
@@ -1,78 +1,108 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>response</t>
-  </si>
-  <si>
-    <t>ayo@xmail.com</t>
-  </si>
-  <si>
-    <t>ayo123</t>
-  </si>
-  <si>
-    <t>valid</t>
-  </si>
-  <si>
-    <t>sambezoz@tmail.com</t>
-  </si>
-  <si>
-    <t>JJu(*&amp;ff+_</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>zayidjarrah@hmail.com</t>
-  </si>
-  <si>
-    <t>:LKJHA978y</t>
-  </si>
-  <si>
-    <t>kateausten@qmail.com</t>
-  </si>
-  <si>
-    <t>)(*A^&amp;osdijh</t>
-  </si>
-  <si>
-    <t>jacobsmith@zmail.com</t>
-  </si>
-  <si>
-    <t>t3$7pwD#O07</t>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ayo@xmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ayo123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sambezoz@tmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JJu(*&amp;ff+_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zayidjarrah@hmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:LKJHA978y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kateausten@qmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">)(*A^&amp;osdijh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jacobsmith@zmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3$7pwD#O07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -80,7 +110,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -90,59 +120,80 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -153,94 +204,90 @@
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4285f4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ea4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="fbbc04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="34a853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="ff6d01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="46bdc6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -248,33 +295,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -287,13 +325,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -303,15 +335,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -319,7 +349,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -327,11 +356,11 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -340,21 +369,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.13"/>
-    <col customWidth="1" min="2" max="2" width="17.88"/>
-    <col customWidth="1" min="3" max="3" width="14.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.75"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -365,7 +397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -376,7 +408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -387,7 +419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -395,10 +427,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -409,7 +441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -421,6 +453,12 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added testngGrouping.xml file, and added groups to every test method.
</commit_message>
<xml_diff>
--- a/testdata/OpenCart_LoginData.xlsx
+++ b/testdata/OpenCart_LoginData.xlsx
@@ -167,20 +167,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,80 +380,80 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>